<commit_message>
adding activity tracker to the register new company page
</commit_message>
<xml_diff>
--- a/invoice_gen/TEMPLATE/JLFMH.xlsx
+++ b/invoice_gen/TEMPLATE/JLFMH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\tools\inv_pkl_contract_creation - Copy\invoice_gen\TEMPLATE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\GENERATE_INVOICE_STREAMLIT_WEB\invoice_gen\TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C926185-CB00-42B7-8CDA-759FFB088DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF2DAAE-5A79-4152-835C-6AD77DA5E2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="6" r:id="rId1"/>
@@ -110,12 +110,6 @@
     <t>Timberland Co.,Ltd</t>
   </si>
   <si>
-    <t>P+84 989 777 156  Contact: Mai Ca    Email:vn01@rm-motion.com,and Vn-custom03@manwahgroup.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Postcode: 820000   TAX ID: 3700762351</t>
-  </si>
-  <si>
     <t xml:space="preserve">SHIP: </t>
   </si>
   <si>
@@ -259,13 +253,19 @@
     <t>JFTIME</t>
   </si>
   <si>
-    <t xml:space="preserve"> No. 35, Group 2, Binh Chanh Quarter, Tan Hiep Ward, Ho Chi Minh city, Vietnam.</t>
-  </si>
-  <si>
     <t>HCM</t>
   </si>
   <si>
     <t>BY TRUCK FROM BAVET, SVAY RIENG, CAMBODIA TO HO CHI MINH CITY, VIETNAM.</t>
+  </si>
+  <si>
+    <t>No. 345, Map sheet no. 35, Group 2, Phuoc Chanh Quarter, Tan Hiep Ward, Ho Chi Minh City Viet Nam.</t>
+  </si>
+  <si>
+    <t>Tax ID code: 3700762351 Postcode: 820000 Contact: Ms.Mai Ca</t>
+  </si>
+  <si>
+    <t>Cell phone: 84 989 777 156 Email: Vn-custom03@manwahgroup.com</t>
   </si>
 </sst>
 </file>
@@ -694,6 +694,21 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -706,19 +721,20 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -733,22 +749,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1213,91 +1213,91 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="7.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" style="41" customWidth="1"/>
-    <col min="8" max="8" width="25.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" customWidth="1"/>
-    <col min="16" max="23" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="4" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" customWidth="1"/>
+    <col min="7" max="7" width="26.5546875" style="41" customWidth="1"/>
+    <col min="8" max="8" width="25.109375" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" customWidth="1"/>
+    <col min="15" max="15" width="16.109375" customWidth="1"/>
+    <col min="16" max="23" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="38.25" customHeight="1">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
     </row>
     <row r="2" spans="1:7" ht="24" customHeight="1">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
     </row>
     <row r="3" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
     </row>
     <row r="4" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
     </row>
     <row r="6" spans="1:7" ht="83.25" customHeight="1">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1">
       <c r="A7" s="39"/>
@@ -1309,7 +1309,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="39" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1">
@@ -1325,7 +1325,7 @@
         <v>8</v>
       </c>
       <c r="G8" s="46" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" customHeight="1">
@@ -1339,7 +1339,7 @@
         <v>10</v>
       </c>
       <c r="G9" s="33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="22.5" customHeight="1">
@@ -1353,7 +1353,7 @@
         <v>12</v>
       </c>
       <c r="G10" s="48" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="20.25" customHeight="1">
@@ -1370,7 +1370,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.95" customHeight="1">
+    <row r="12" spans="1:7" ht="18.899999999999999" customHeight="1">
       <c r="A12" s="39"/>
       <c r="B12" s="39"/>
       <c r="C12" s="39"/>
@@ -1405,7 +1405,7 @@
     <row r="15" spans="1:7" ht="25.5" customHeight="1">
       <c r="A15" s="39"/>
       <c r="B15" s="15" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1415,7 +1415,7 @@
     <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="39"/>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1430,10 +1430,10 @@
     </row>
     <row r="18" spans="1:23" ht="27.75" customHeight="1">
       <c r="A18" s="52" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C18" s="53"/>
       <c r="D18" s="1"/>
@@ -1482,61 +1482,61 @@
       <c r="G22" s="51"/>
     </row>
     <row r="23" spans="1:23" ht="42" customHeight="1">
-      <c r="A23" s="69" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
-      <c r="D23" s="69"/>
+      <c r="A23" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
       <c r="E23" s="39"/>
       <c r="F23" s="39"/>
       <c r="G23" s="42"/>
     </row>
     <row r="24" spans="1:23" ht="61.5" customHeight="1">
       <c r="A24" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="70" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" s="70"/>
-      <c r="D24" s="70"/>
+        <v>19</v>
+      </c>
+      <c r="B24" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="66"/>
+      <c r="D24" s="66"/>
       <c r="E24" s="57"/>
       <c r="F24" s="39"/>
       <c r="G24" s="42"/>
     </row>
     <row r="25" spans="1:23" ht="42" customHeight="1">
-      <c r="A25" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="71"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="71"/>
+      <c r="A25" s="67" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
       <c r="E25" s="58"/>
       <c r="F25" s="58"/>
       <c r="G25" s="42"/>
     </row>
     <row r="26" spans="1:23" ht="24.75" customHeight="1">
-      <c r="A26" s="67" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="67"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="67"/>
+      <c r="A26" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="63"/>
     </row>
     <row r="27" spans="1:23" s="40" customFormat="1" ht="27" customHeight="1">
-      <c r="A27" s="67" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="67"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="67"/>
-      <c r="G27" s="67"/>
+      <c r="A27" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="63"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
     </row>
     <row r="28" spans="1:23" ht="42" customHeight="1">
       <c r="E28" s="47"/>
@@ -1548,7 +1548,7 @@
     <row r="29" spans="1:23" ht="24" customHeight="1">
       <c r="E29" s="39"/>
       <c r="F29" s="60" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="42" customHeight="1">
@@ -1558,7 +1558,7 @@
     <row r="31" spans="1:23" ht="53.1" customHeight="1">
       <c r="E31" s="39"/>
       <c r="F31" s="61" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G31" s="62"/>
     </row>
@@ -1584,17 +1584,17 @@
     <row r="62" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="A23:D23"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="A25:D25"/>
     <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
   </mergeCells>
   <conditionalFormatting sqref="J23:J34">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
@@ -1614,122 +1614,122 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A2" zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="7.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22" style="4" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="4" customWidth="1"/>
-    <col min="3" max="4" width="15.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="4" customWidth="1"/>
-    <col min="8" max="10" width="16.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="15.88671875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" style="4" customWidth="1"/>
+    <col min="8" max="10" width="16.5546875" style="4" customWidth="1"/>
     <col min="11" max="11" width="15" style="4" customWidth="1"/>
     <col min="12" max="12" width="10" style="4" customWidth="1"/>
-    <col min="13" max="13" width="25.140625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" style="4" customWidth="1"/>
-    <col min="16" max="16" width="7.140625" style="4"/>
-    <col min="17" max="17" width="12.42578125" style="4" customWidth="1"/>
-    <col min="18" max="16384" width="7.140625" style="4"/>
+    <col min="13" max="13" width="25.109375" style="4" customWidth="1"/>
+    <col min="14" max="14" width="15.5546875" style="4" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="7.109375" style="4"/>
+    <col min="17" max="17" width="12.44140625" style="4" customWidth="1"/>
+    <col min="18" max="16384" width="7.109375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="38.25" customHeight="1">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
       <c r="K1" s="28"/>
       <c r="L1" s="28"/>
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1">
-      <c r="A2" s="73" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
+      <c r="A2" s="79" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
     <row r="3" spans="1:12" ht="25.5" customHeight="1">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
       <c r="K3" s="27"/>
       <c r="L3" s="27"/>
     </row>
     <row r="4" spans="1:12" ht="25.5" customHeight="1">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
       <c r="K4" s="27"/>
       <c r="L4" s="27"/>
     </row>
     <row r="5" spans="1:12" ht="25.5" customHeight="1">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
       <c r="K5" s="27"/>
       <c r="L5" s="27"/>
     </row>
     <row r="6" spans="1:12" ht="54" customHeight="1">
-      <c r="A6" s="76" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="76"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="76"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="76"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="76"/>
-      <c r="I6" s="76"/>
-      <c r="J6" s="76"/>
+      <c r="A6" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
       <c r="K6" s="29"/>
       <c r="L6" s="29"/>
     </row>
@@ -1746,7 +1746,7 @@
         <v>6</v>
       </c>
       <c r="J7" s="30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
@@ -1764,7 +1764,7 @@
         <v>8</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="21" customHeight="1">
@@ -1780,13 +1780,13 @@
         <v>10</v>
       </c>
       <c r="J9" s="33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="22.5" customHeight="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1797,7 +1797,7 @@
         <v>DAP:</v>
       </c>
       <c r="J10" s="34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K10" s="35"/>
     </row>
@@ -1813,7 +1813,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="24.95" customHeight="1">
+    <row r="12" spans="1:12" ht="24.9" customHeight="1">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1862,7 +1862,7 @@
     <row r="15" spans="1:12" ht="25.5" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" s="15" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
@@ -1875,10 +1875,10 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" ht="21.95" customHeight="1">
+    <row r="16" spans="1:12" ht="21.9" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -1893,37 +1893,37 @@
     </row>
     <row r="17" spans="1:13" ht="27.75" customHeight="1">
       <c r="A17" s="16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:13" ht="18.95" customHeight="1">
+    <row r="18" spans="1:13" ht="18.899999999999999" customHeight="1">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
     </row>
-    <row r="19" spans="1:13" ht="18.95" customHeight="1">
+    <row r="19" spans="1:13" ht="18.899999999999999" customHeight="1">
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
     </row>
-    <row r="20" spans="1:13" ht="18.95" customHeight="1">
+    <row r="20" spans="1:13" ht="18.899999999999999" customHeight="1">
       <c r="A20" s="17"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
     </row>
-    <row r="21" spans="1:13" ht="18.95" customHeight="1">
+    <row r="21" spans="1:13" ht="18.899999999999999" customHeight="1">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -1944,14 +1944,14 @@
       <c r="M22" s="36"/>
     </row>
     <row r="23" spans="1:13" ht="42" customHeight="1">
-      <c r="A23" s="77" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="77"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
+      <c r="A23" s="75" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
       <c r="G23" s="23"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -1962,15 +1962,15 @@
     </row>
     <row r="24" spans="1:13" ht="61.5" customHeight="1">
       <c r="A24" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="78" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" s="78"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="78"/>
+        <v>19</v>
+      </c>
+      <c r="B24" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="76"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="76"/>
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
       <c r="I24" s="25"/>
@@ -1980,14 +1980,14 @@
       <c r="M24" s="37"/>
     </row>
     <row r="25" spans="1:13" ht="44.1" customHeight="1">
-      <c r="A25" s="79" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="79"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="79"/>
-      <c r="E25" s="79"/>
-      <c r="F25" s="79"/>
+      <c r="A25" s="77" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="77"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="77"/>
       <c r="G25" s="26"/>
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
@@ -1997,36 +1997,36 @@
       <c r="M25" s="37"/>
     </row>
     <row r="26" spans="1:13" ht="24.75" customHeight="1">
-      <c r="A26" s="80" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="80"/>
-      <c r="C26" s="80"/>
-      <c r="D26" s="80"/>
-      <c r="E26" s="80"/>
-      <c r="F26" s="80"/>
-      <c r="G26" s="80"/>
-      <c r="H26" s="80"/>
-      <c r="I26" s="80"/>
-      <c r="J26" s="80"/>
-      <c r="K26" s="80"/>
-      <c r="L26" s="80"/>
+      <c r="A26" s="72" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="72"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="72"/>
+      <c r="J26" s="72"/>
+      <c r="K26" s="72"/>
+      <c r="L26" s="72"/>
     </row>
     <row r="27" spans="1:13" s="3" customFormat="1" ht="27" customHeight="1">
-      <c r="A27" s="80" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="80"/>
-      <c r="C27" s="80"/>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="80"/>
-      <c r="G27" s="80"/>
-      <c r="H27" s="80"/>
-      <c r="I27" s="80"/>
-      <c r="J27" s="80"/>
-      <c r="K27" s="80"/>
-      <c r="L27" s="80"/>
+      <c r="A27" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="72"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="72"/>
+      <c r="K27" s="72"/>
+      <c r="L27" s="72"/>
     </row>
     <row r="28" spans="1:13" ht="42" customHeight="1">
       <c r="H28" s="12" t="s">
@@ -2050,8 +2050,8 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="81"/>
-      <c r="L31" s="81"/>
+      <c r="K31" s="73"/>
+      <c r="L31" s="73"/>
     </row>
     <row r="32" spans="1:13" ht="53.1" customHeight="1">
       <c r="H32" s="5"/>
@@ -2081,6 +2081,11 @@
     <row r="63" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:J5"/>
     <mergeCell ref="A27:L27"/>
     <mergeCell ref="K31:L31"/>
     <mergeCell ref="A6:J6"/>
@@ -2088,11 +2093,6 @@
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="A25:F25"/>
     <mergeCell ref="A26:L26"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A5:J5"/>
   </mergeCells>
   <conditionalFormatting sqref="O23:O35">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
@@ -2113,7 +2113,7 @@
       <selection activeCell="S94" sqref="S94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>

</xml_diff>